<commit_message>
feat: adds sidekick foo plugin.
</commit_message>
<xml_diff>
--- a/tools/sidekick/libarary.xlsx
+++ b/tools/sidekick/libarary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dasilrui/Projects/diconium/adobe/aem-site/tools/sidekick/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2763EF89-DE29-364C-853C-7EEC85833D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AC2636-8077-1143-8E39-74E6B11BFF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14060" yWindow="740" windowWidth="13840" windowHeight="29780" xr2:uid="{BFAFEA3A-05C5-B645-8C7B-A6A5B9BF8CB9}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <t>path</t>
   </si>
   <si>
-    <t>https://main--aem-site--lopesdasilva.hlx.live/tools/sidekick/foo</t>
+    <t>https://main--aem-site--lopesdasilva.hlx.live/tools/sidekick/foo.html</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>